<commit_message>
Add payment 76442781 (Cash) 2025-08-15T09:33:31
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,10 +456,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A2" t="n">
+        <v>76442781</v>
       </c>
       <c r="B2" t="n">
         <v>85</v>
@@ -472,6 +470,26 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>2025-08-15T09:33:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>95</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-08-15T09:33:31</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71652621 (Cash) 2025-08-15T09:33:45
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,10 +474,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A3" t="n">
+        <v>76442781</v>
       </c>
       <c r="B3" t="n">
         <v>95</v>
@@ -490,6 +488,26 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>2025-08-15T09:33:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>71652621</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-08-15T09:33:45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71652621 (Cash) 2025-08-15T09:33:54
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,10 +492,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>71652621</t>
-        </is>
+      <c r="A4" t="n">
+        <v>71652621</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -508,6 +506,26 @@
       <c r="D4" t="inlineStr">
         <is>
           <t>2025-08-15T09:33:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>71652621</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>71</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-08-15T09:33:54</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71652621 (Cash) 2025-08-15T09:35:01
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,10 +510,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>71652621</t>
-        </is>
+      <c r="A5" t="n">
+        <v>71652621</v>
       </c>
       <c r="B5" t="n">
         <v>71</v>
@@ -526,6 +524,26 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>2025-08-15T09:33:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>71652621</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>71</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-08-15T09:35:01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71652621 (Cash) 2025-08-15T09:47:50
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,10 +528,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>71652621</t>
-        </is>
+      <c r="A6" t="n">
+        <v>71652621</v>
       </c>
       <c r="B6" t="n">
         <v>71</v>
@@ -544,6 +542,26 @@
       <c r="D6" t="inlineStr">
         <is>
           <t>2025-08-15T09:35:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>71652621</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>20</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-08-15T09:47:50</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 76442781 (Cash) 2025-08-15T09:48:27
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,10 +546,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>71652621</t>
-        </is>
+      <c r="A7" t="n">
+        <v>71652621</v>
       </c>
       <c r="B7" t="n">
         <v>20</v>
@@ -562,6 +560,26 @@
       <c r="D7" t="inlineStr">
         <is>
           <t>2025-08-15T09:47:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>20</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-08-15T09:48:27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 76442780 (Cash) 2025-08-15T09:54:44
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,10 +564,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A8" t="n">
+        <v>76442781</v>
       </c>
       <c r="B8" t="n">
         <v>20</v>
@@ -580,6 +578,26 @@
       <c r="D8" t="inlineStr">
         <is>
           <t>2025-08-15T09:48:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>76442780</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>17</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-08-15T09:54:44</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 76442780 (Cash) 2025-08-15T09:55:46
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,10 +582,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>76442780</t>
-        </is>
+      <c r="A9" t="n">
+        <v>76442780</v>
       </c>
       <c r="B9" t="n">
         <v>17</v>
@@ -598,6 +596,26 @@
       <c r="D9" t="inlineStr">
         <is>
           <t>2025-08-15T09:54:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>76442780</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>170</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-08-15T09:55:46</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 76442780 (Cash) 2025-08-15T10:00:21
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,21 @@
           <t>timestamp</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>original_amount</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>discount_applied</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>final_amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -472,6 +487,9 @@
           <t>2025-08-15T09:33:10</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -490,6 +508,9 @@
           <t>2025-08-15T09:33:31</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -508,6 +529,9 @@
           <t>2025-08-15T09:33:45</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -526,6 +550,9 @@
           <t>2025-08-15T09:33:54</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -544,6 +571,9 @@
           <t>2025-08-15T09:35:01</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -562,6 +592,9 @@
           <t>2025-08-15T09:47:50</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -580,6 +613,9 @@
           <t>2025-08-15T09:48:27</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -598,12 +634,13 @@
           <t>2025-08-15T09:54:44</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>76442780</t>
-        </is>
+      <c r="A10" t="n">
+        <v>76442780</v>
       </c>
       <c r="B10" t="n">
         <v>170</v>
@@ -617,6 +654,36 @@
         <is>
           <t>2025-08-15T09:55:46</t>
         </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>76442780</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-08-15T10:00:21</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>200</v>
+      </c>
+      <c r="F11" t="n">
+        <v>30</v>
+      </c>
+      <c r="G11" t="n">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 76442780 (Cash) 2025-08-15T10:00:30
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,10 +660,8 @@
       <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>76442780</t>
-        </is>
+      <c r="A11" t="n">
+        <v>76442780</v>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
@@ -683,6 +681,33 @@
         <v>30</v>
       </c>
       <c r="G11" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>76442780</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-08-15T10:00:30</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>200</v>
+      </c>
+      <c r="F12" t="n">
+        <v>30</v>
+      </c>
+      <c r="G12" t="n">
         <v>170</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79172233 (Credit Card) 2025-08-18T08:33:09
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -685,10 +685,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>76442780</t>
-        </is>
+      <c r="A12" t="n">
+        <v>76442780</v>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
@@ -709,6 +707,33 @@
       </c>
       <c r="G12" t="n">
         <v>170</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>79172233</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Credit Card</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-08-18T08:33:09</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>30</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T08:41:43
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,16 @@
           <t>final_amount</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>birthday_discount</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>points_redeemed</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -490,6 +500,8 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -511,6 +523,8 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -532,6 +546,8 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -553,6 +569,8 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -574,6 +592,8 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -595,6 +615,8 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -616,6 +638,8 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -637,6 +661,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -658,6 +684,8 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -683,6 +711,8 @@
       <c r="G11" t="n">
         <v>170</v>
       </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -708,12 +738,12 @@
       <c r="G12" t="n">
         <v>170</v>
       </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>79172233</t>
-        </is>
+      <c r="A13" t="n">
+        <v>79172233</v>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
@@ -734,6 +764,39 @@
       </c>
       <c r="G13" t="n">
         <v>30</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-08-18T08:41:43</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>20</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>20</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T08:46:52
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -769,10 +769,8 @@
       <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A14" t="n">
+        <v>79174445</v>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
@@ -797,6 +795,37 @@
       </c>
       <c r="I14" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-08-18T08:46:52</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>30</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>10</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T08:51:16
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -798,10 +798,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A15" t="n">
+        <v>79174445</v>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
@@ -826,6 +824,37 @@
       </c>
       <c r="I15" t="n">
         <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-08-18T08:51:16</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>40</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>10</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T08:51:52
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -827,10 +827,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A16" t="n">
+        <v>79174445</v>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
@@ -855,6 +853,37 @@
       </c>
       <c r="I16" t="n">
         <v>30</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-08-18T08:51:52</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>20</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T08:51:56
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -856,10 +856,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A17" t="n">
+        <v>79174445</v>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
@@ -883,6 +881,37 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-08-18T08:51:56</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>20</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T08:57:38
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -885,10 +885,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A18" t="n">
+        <v>79174445</v>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
@@ -913,6 +911,37 @@
       </c>
       <c r="I18" t="n">
         <v>20</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-08-18T08:57:38</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>30</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T09:08:11
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -914,10 +914,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A19" t="n">
+        <v>79174445</v>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
@@ -942,6 +940,37 @@
       </c>
       <c r="I19" t="n">
         <v>30</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-08-18T09:08:11</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>20</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277628 (Cash) 2025-08-18T16:53:13
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -943,10 +943,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A20" t="n">
+        <v>79174445</v>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
@@ -971,6 +969,37 @@
       </c>
       <c r="I20" t="n">
         <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:53:13</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>80</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="n">
+        <v>80</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277628 (Cash) 2025-08-18T16:53:26
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -972,10 +972,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A21" t="n">
+        <v>71277628</v>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
@@ -1000,6 +998,37 @@
       </c>
       <c r="I21" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:53:26</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>800</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>720</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277628 (Cash) 2025-08-18T16:53:40
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1001,10 +1001,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A22" t="n">
+        <v>71277628</v>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
@@ -1029,6 +1027,37 @@
       </c>
       <c r="I22" t="n">
         <v>80</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:53:40</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>760</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>760</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277628 (Cash) 2025-08-18T16:53:54
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1030,10 +1030,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A23" t="n">
+        <v>71277628</v>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
@@ -1058,6 +1056,37 @@
       </c>
       <c r="I23" t="n">
         <v>760</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:53:54</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>766</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277628 (Cash) 2025-08-18T16:54:29
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1059,10 +1059,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A24" t="n">
+        <v>71277628</v>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
@@ -1086,6 +1084,37 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:54:29</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>766</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
         <v>766</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71277628 (Cash) 2025-08-18T16:54:45
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1088,10 +1088,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A25" t="n">
+        <v>71277628</v>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
@@ -1116,6 +1114,37 @@
       </c>
       <c r="I25" t="n">
         <v>766</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:54:45</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>76</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277628 (Cash) 2025-08-18T16:54:50
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1117,10 +1117,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A26" t="n">
+        <v>71277628</v>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
@@ -1144,6 +1142,37 @@
         <v>0</v>
       </c>
       <c r="I26" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:54:50</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>76</v>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71277628 (Cash) 2025-08-18T16:54:54
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1146,10 +1146,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A27" t="n">
+        <v>71277628</v>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
@@ -1173,6 +1171,37 @@
         <v>0</v>
       </c>
       <c r="I27" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:54:54</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>76</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:04:07
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1175,10 +1175,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A28" t="n">
+        <v>71277628</v>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
@@ -1203,6 +1201,37 @@
       </c>
       <c r="I28" t="n">
         <v>76</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:04:07</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>76</v>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="n">
+        <v>76</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:04:15
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1204,10 +1204,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A29" t="n">
+        <v>71277620</v>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
@@ -1232,6 +1230,37 @@
       </c>
       <c r="I29" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:04:15</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>760</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>684</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:04:26
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1233,10 +1233,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A30" t="n">
+        <v>71277620</v>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
@@ -1261,6 +1259,37 @@
       </c>
       <c r="I30" t="n">
         <v>76</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:04:26</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>760</v>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>760</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:04:40
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1262,10 +1262,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A31" t="n">
+        <v>71277620</v>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
@@ -1290,6 +1288,37 @@
       </c>
       <c r="I31" t="n">
         <v>760</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:04:40</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>76</v>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:10:03
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1291,10 +1291,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A32" t="n">
+        <v>71277620</v>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
@@ -1319,6 +1317,37 @@
       </c>
       <c r="I32" t="n">
         <v>76</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:10:03</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>76</v>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="n">
+        <v>76</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:10:08
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1320,10 +1320,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A33" t="n">
+        <v>71277620</v>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
@@ -1347,6 +1345,37 @@
         <v>0</v>
       </c>
       <c r="I33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:10:08</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>76</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="n">
+        <v>76</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:10:20
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1349,10 +1349,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A34" t="n">
+        <v>71277620</v>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
@@ -1377,6 +1375,37 @@
       </c>
       <c r="I34" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:10:20</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>76</v>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:10:26
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1378,10 +1378,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A35" t="n">
+        <v>71277620</v>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
@@ -1405,6 +1403,37 @@
         <v>0</v>
       </c>
       <c r="I35" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:10:26</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>76</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:11:19
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1407,10 +1407,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A36" t="n">
+        <v>71277620</v>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
@@ -1435,6 +1433,37 @@
       </c>
       <c r="I36" t="n">
         <v>76</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:11:19</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>76</v>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="n">
+        <v>76</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:28:47
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1436,10 +1436,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A37" t="n">
+        <v>71277620</v>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
@@ -1463,6 +1461,37 @@
         <v>0</v>
       </c>
       <c r="I37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:28:47</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>76</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="n">
+        <v>76</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:28:56
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1465,10 +1465,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A38" t="n">
+        <v>71277620</v>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
@@ -1493,6 +1491,37 @@
       </c>
       <c r="I38" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:28:56</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>76</v>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:29:17
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1494,10 +1494,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A39" t="n">
+        <v>71277620</v>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
@@ -1522,6 +1520,37 @@
       </c>
       <c r="I39" t="n">
         <v>76</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:29:17</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>100</v>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="n">
+        <v>100</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71277620 (Cash) 2025-08-18T17:29:26
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1523,10 +1523,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A40" t="n">
+        <v>71277620</v>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
@@ -1551,6 +1549,37 @@
       </c>
       <c r="I40" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:29:26</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>100</v>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T17:42:14
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1552,10 +1552,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A41" t="n">
+        <v>71277620</v>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
@@ -1580,6 +1578,37 @@
       </c>
       <c r="I41" t="n">
         <v>100</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:42:14</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>60</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="n">
+        <v>60</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T17:42:49
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1581,10 +1581,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A42" t="n">
+        <v>79174445</v>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
@@ -1608,6 +1606,37 @@
         <v>0</v>
       </c>
       <c r="I42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:42:49</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>60</v>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="n">
+        <v>60</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T17:42:58
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1610,10 +1610,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A43" t="n">
+        <v>79174445</v>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
@@ -1637,6 +1635,37 @@
         <v>0</v>
       </c>
       <c r="I43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:42:58</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>60</v>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="n">
+        <v>60</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T17:43:02
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1639,10 +1639,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A44" t="n">
+        <v>79174445</v>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
@@ -1666,6 +1664,37 @@
         <v>0</v>
       </c>
       <c r="I44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:43:02</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>60</v>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="n">
+        <v>60</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T17:43:07
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1668,10 +1668,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A45" t="n">
+        <v>79174445</v>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
@@ -1695,6 +1693,37 @@
         <v>0</v>
       </c>
       <c r="I45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:43:07</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>600</v>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="n">
+        <v>600</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T17:43:44
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1697,10 +1697,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A46" t="n">
+        <v>79174445</v>
       </c>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
@@ -1724,6 +1722,37 @@
         <v>0</v>
       </c>
       <c r="I46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:43:44</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>20</v>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="n">
+        <v>20</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-18T17:46:33
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1726,10 +1726,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A47" t="n">
+        <v>79174445</v>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
@@ -1753,6 +1751,37 @@
         <v>0</v>
       </c>
       <c r="I47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:46:33</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>200</v>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="n">
+        <v>200</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71076783 (Cash) 2025-08-18T17:49:44
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1755,10 +1755,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A48" t="n">
+        <v>79174445</v>
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
@@ -1782,6 +1780,37 @@
         <v>0</v>
       </c>
       <c r="I48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>71076783</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:49:44</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>200</v>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="n">
+        <v>200</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71076783 (Cash) 2025-08-18T17:51:54
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1784,10 +1784,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>71076783</t>
-        </is>
+      <c r="A49" t="n">
+        <v>71076783</v>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr">
@@ -1811,6 +1809,37 @@
         <v>0</v>
       </c>
       <c r="I49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>71076783</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:51:54</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>120</v>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="n">
+        <v>120</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71076783 (Cash) 2025-08-18T18:01:45
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>points_redeemed</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>reward_discount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -502,6 +507,9 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -525,6 +533,9 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -548,6 +559,9 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -571,6 +585,9 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -594,6 +611,9 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -617,6 +637,9 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -640,6 +663,9 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -663,6 +689,9 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -686,6 +715,9 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -713,6 +745,9 @@
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -740,6 +775,9 @@
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -767,6 +805,9 @@
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -796,6 +837,9 @@
       <c r="I14" t="n">
         <v>0</v>
       </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -825,6 +869,9 @@
       <c r="I15" t="n">
         <v>20</v>
       </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -854,6 +901,9 @@
       <c r="I16" t="n">
         <v>30</v>
       </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -883,6 +933,9 @@
       <c r="I17" t="n">
         <v>20</v>
       </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -912,6 +965,9 @@
       <c r="I18" t="n">
         <v>20</v>
       </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -941,6 +997,9 @@
       <c r="I19" t="n">
         <v>30</v>
       </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -970,6 +1029,9 @@
       <c r="I20" t="n">
         <v>20</v>
       </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -999,6 +1061,9 @@
       <c r="I21" t="n">
         <v>0</v>
       </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1028,6 +1093,9 @@
       <c r="I22" t="n">
         <v>80</v>
       </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1057,6 +1125,9 @@
       <c r="I23" t="n">
         <v>760</v>
       </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1086,6 +1157,9 @@
       <c r="I24" t="n">
         <v>766</v>
       </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1115,6 +1189,9 @@
       <c r="I25" t="n">
         <v>766</v>
       </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1144,6 +1221,9 @@
       <c r="I26" t="n">
         <v>76</v>
       </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1173,6 +1253,9 @@
       <c r="I27" t="n">
         <v>76</v>
       </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1202,6 +1285,9 @@
       <c r="I28" t="n">
         <v>76</v>
       </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1231,6 +1317,9 @@
       <c r="I29" t="n">
         <v>0</v>
       </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1260,6 +1349,9 @@
       <c r="I30" t="n">
         <v>76</v>
       </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1289,6 +1381,9 @@
       <c r="I31" t="n">
         <v>760</v>
       </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1318,6 +1413,9 @@
       <c r="I32" t="n">
         <v>76</v>
       </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1347,6 +1445,9 @@
       <c r="I33" t="n">
         <v>0</v>
       </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1376,6 +1477,9 @@
       <c r="I34" t="n">
         <v>0</v>
       </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1405,6 +1509,9 @@
       <c r="I35" t="n">
         <v>76</v>
       </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1434,6 +1541,9 @@
       <c r="I36" t="n">
         <v>76</v>
       </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1463,6 +1573,9 @@
       <c r="I37" t="n">
         <v>0</v>
       </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1492,6 +1605,9 @@
       <c r="I38" t="n">
         <v>0</v>
       </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1521,6 +1637,9 @@
       <c r="I39" t="n">
         <v>76</v>
       </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1550,6 +1669,9 @@
       <c r="I40" t="n">
         <v>0</v>
       </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1579,6 +1701,9 @@
       <c r="I41" t="n">
         <v>100</v>
       </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1608,6 +1733,9 @@
       <c r="I42" t="n">
         <v>0</v>
       </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1637,6 +1765,9 @@
       <c r="I43" t="n">
         <v>0</v>
       </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1666,6 +1797,9 @@
       <c r="I44" t="n">
         <v>0</v>
       </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1695,6 +1829,9 @@
       <c r="I45" t="n">
         <v>0</v>
       </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1724,6 +1861,9 @@
       <c r="I46" t="n">
         <v>0</v>
       </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1753,6 +1893,9 @@
       <c r="I47" t="n">
         <v>0</v>
       </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1782,6 +1925,9 @@
       <c r="I48" t="n">
         <v>0</v>
       </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1811,12 +1957,13 @@
       <c r="I49" t="n">
         <v>0</v>
       </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>71076783</t>
-        </is>
+      <c r="A50" t="n">
+        <v>71076783</v>
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr">
@@ -1841,6 +1988,43 @@
       </c>
       <c r="I50" t="n">
         <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>71076783</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:01:45</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>120</v>
+      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="n">
+        <v>115</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>100</v>
+      </c>
+      <c r="J51" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 09876543 (Cash) 2025-08-18T18:03:03
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1994,10 +1994,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>71076783</t>
-        </is>
+      <c r="A51" t="n">
+        <v>71076783</v>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
@@ -2025,6 +2023,40 @@
       </c>
       <c r="J51" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>09876543</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:03:03</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>120</v>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="n">
+        <v>120</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 09876543 (Cash) 2025-08-18T18:03:23
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2026,10 +2026,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>09876543</t>
-        </is>
+      <c r="A52" t="n">
+        <v>9876543</v>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr">
@@ -2056,6 +2054,40 @@
         <v>0</v>
       </c>
       <c r="J52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>09876543</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:03:23</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>120</v>
+      </c>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="n">
+        <v>120</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 09876543 (Cash) 2025-08-18T18:03:44
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2058,10 +2058,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>09876543</t>
-        </is>
+      <c r="A53" t="n">
+        <v>9876543</v>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr">
@@ -2088,6 +2086,40 @@
         <v>0</v>
       </c>
       <c r="J53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>09876543</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:03:44</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>120</v>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="n">
+        <v>120</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 09876543 (Cash) 2025-08-18T18:04:18
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2090,10 +2090,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>09876543</t>
-        </is>
+      <c r="A54" t="n">
+        <v>9876543</v>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr">
@@ -2120,6 +2118,40 @@
         <v>0</v>
       </c>
       <c r="J54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>09876543</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:04:18</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>120</v>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="n">
+        <v>120</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 09876543 (Cash) 2025-08-18T18:04:40
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2122,10 +2122,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>09876543</t>
-        </is>
+      <c r="A55" t="n">
+        <v>9876543</v>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
@@ -2152,6 +2150,40 @@
         <v>0</v>
       </c>
       <c r="J55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>09876543</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:04:40</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>120</v>
+      </c>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="n">
+        <v>120</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 09876543 (Cash) 2025-08-18T18:05:43
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2154,10 +2154,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>09876543</t>
-        </is>
+      <c r="A56" t="n">
+        <v>9876543</v>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
@@ -2184,6 +2182,40 @@
         <v>0</v>
       </c>
       <c r="J56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>09876543</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:05:43</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>120</v>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="n">
+        <v>120</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 76442781 (Cash) 2025-08-18T18:06:01
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2186,10 +2186,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>09876543</t>
-        </is>
+      <c r="A57" t="n">
+        <v>9876543</v>
       </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
@@ -2216,6 +2214,40 @@
         <v>0</v>
       </c>
       <c r="J57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:06:01</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>120</v>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="n">
+        <v>120</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 76442781 (Cash) 2025-08-18T18:06:34
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2218,10 +2218,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A58" t="n">
+        <v>76442781</v>
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
@@ -2249,6 +2247,40 @@
       </c>
       <c r="J58" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:06:34</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>120</v>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>115</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>100</v>
+      </c>
+      <c r="J59" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 76442781 (Cash) 2025-08-18T18:07:47
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2250,10 +2250,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A59" t="n">
+        <v>76442781</v>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr">
@@ -2281,6 +2279,40 @@
       </c>
       <c r="J59" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:07:47</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>120</v>
+      </c>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="n">
+        <v>120</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 76442781 (Cash) 2025-08-18T18:08:21
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2282,10 +2282,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A60" t="n">
+        <v>76442781</v>
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr">
@@ -2313,6 +2311,40 @@
       </c>
       <c r="J60" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:08:21</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>120</v>
+      </c>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="n">
+        <v>105</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>250</v>
+      </c>
+      <c r="J61" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 51616172 (Cash) 2025-08-20T07:32:19
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2314,10 +2314,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A61" t="n">
+        <v>76442781</v>
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr">
@@ -2345,6 +2343,40 @@
       </c>
       <c r="J61" t="n">
         <v>15</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>51616172</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2025-08-20T07:32:19</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>120</v>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="n">
+        <v>120</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 51616176 (Cash) 2025-08-20T07:33:39
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2346,10 +2346,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>51616172</t>
-        </is>
+      <c r="A62" t="n">
+        <v>51616172</v>
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
@@ -2376,6 +2374,40 @@
         <v>0</v>
       </c>
       <c r="J62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>51616176</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2025-08-20T07:33:39</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>125</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="n">
+        <v>125</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 51616191 (Cash) 2025-08-20T08:04:15
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2378,10 +2378,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>51616176</t>
-        </is>
+      <c r="A63" t="n">
+        <v>51616176</v>
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
@@ -2408,6 +2406,40 @@
         <v>0</v>
       </c>
       <c r="J63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>51616191</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:04:15</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>120</v>
+      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="n">
+        <v>120</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 51616191 (Cash) 2025-08-20T08:04:39
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2410,10 +2410,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>51616191</t>
-        </is>
+      <c r="A64" t="n">
+        <v>51616191</v>
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr">
@@ -2441,6 +2439,40 @@
       </c>
       <c r="J64" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>51616191</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:04:39</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>120</v>
+      </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="n">
+        <v>115</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="n">
+        <v>100</v>
+      </c>
+      <c r="J65" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71717172 (Cash) 2025-08-20T08:11:27
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2442,10 +2442,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>51616191</t>
-        </is>
+      <c r="A65" t="n">
+        <v>51616191</v>
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr">
@@ -2473,6 +2471,40 @@
       </c>
       <c r="J65" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>71717172</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:11:27</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>125</v>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="n">
+        <v>125</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71717170 (Cash) 2025-08-20T08:14:26
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2474,10 +2474,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>71717172</t>
-        </is>
+      <c r="A66" t="n">
+        <v>71717172</v>
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr">
@@ -2504,6 +2502,40 @@
         <v>0</v>
       </c>
       <c r="J66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>71717170</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:14:26</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>127</v>
+      </c>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="n">
+        <v>107.95</v>
+      </c>
+      <c r="H67" t="n">
+        <v>19.05</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71717170 (Cash) 2025-08-20T08:18:12
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2506,10 +2506,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>71717170</t>
-        </is>
+      <c r="A67" t="n">
+        <v>71717170</v>
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr">
@@ -2536,6 +2534,40 @@
         <v>0</v>
       </c>
       <c r="J67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>71717170</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:18:12</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>137</v>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="n">
+        <v>116.45</v>
+      </c>
+      <c r="H68" t="n">
+        <v>20.55</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71717173 (Cash) 2025-08-20T08:22:30
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2538,10 +2538,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>71717170</t>
-        </is>
+      <c r="A68" t="n">
+        <v>71717170</v>
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
@@ -2568,6 +2566,40 @@
         <v>0</v>
       </c>
       <c r="J68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>71717173</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:22:30</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>150</v>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="n">
+        <v>127.5</v>
+      </c>
+      <c r="H69" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 71717173 (Check) 2025-08-20T08:24:26
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2570,10 +2570,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>71717173</t>
-        </is>
+      <c r="A69" t="n">
+        <v>71717173</v>
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr">
@@ -2601,6 +2599,40 @@
       </c>
       <c r="J69" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>71717173</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Check</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:24:26</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>350</v>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="n">
+        <v>292.5</v>
+      </c>
+      <c r="H70" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="I70" t="n">
+        <v>100</v>
+      </c>
+      <c r="J70" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 71717173 (Cash) 2025-08-20T08:25:30
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2602,10 +2602,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>71717173</t>
-        </is>
+      <c r="A70" t="n">
+        <v>71717173</v>
       </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr">
@@ -2633,6 +2631,40 @@
       </c>
       <c r="J70" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>71717173</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:25:30</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>351</v>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="n">
+        <v>298.35</v>
+      </c>
+      <c r="H71" t="n">
+        <v>52.65</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add payment 76442711 (Cash) 2025-08-20T08:42:01
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2634,10 +2634,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>71717173</t>
-        </is>
+      <c r="A71" t="n">
+        <v>71717173</v>
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
@@ -2664,6 +2662,40 @@
         <v>0</v>
       </c>
       <c r="J71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>76442711</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:42:01</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>408</v>
+      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="n">
+        <v>408</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 76442711 (Cash) 2025-08-20T08:43:41
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2666,10 +2666,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>76442711</t>
-        </is>
+      <c r="A72" t="n">
+        <v>76442711</v>
       </c>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr">
@@ -2696,6 +2694,40 @@
         <v>0</v>
       </c>
       <c r="J72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>76442711</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:43:41</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>408</v>
+      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="n">
+        <v>346.8</v>
+      </c>
+      <c r="H73" t="n">
+        <v>61.2</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 76442711 (Cash) 2025-08-20T08:52:14
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,38 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>76442711</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>408</v>
+      </c>
+      <c r="C2" t="n">
+        <v>61.2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>346.8</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:52:14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add payment 76442781 (Cash) 2025-08-20T08:53:29
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,10 +476,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>76442711</t>
-        </is>
+      <c r="A2" t="n">
+        <v>76442711</v>
       </c>
       <c r="B2" t="n">
         <v>408</v>
@@ -504,6 +502,38 @@
       <c r="H2" t="inlineStr">
         <is>
           <t>2025-08-20T08:52:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4080</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4080</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:53:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 76442781 (Check) 2025-08-20T08:55:01
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,10 +506,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A3" t="n">
+        <v>76442781</v>
       </c>
       <c r="B3" t="n">
         <v>4080</v>
@@ -534,6 +532,38 @@
       <c r="H3" t="inlineStr">
         <is>
           <t>2025-08-20T08:53:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>408</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>40</v>
+      </c>
+      <c r="E4" t="n">
+        <v>500</v>
+      </c>
+      <c r="F4" t="n">
+        <v>368</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Check</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:55:01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174463 (Cash) 2025-08-20T09:36:16
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,10 +536,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A4" t="n">
+        <v>76442781</v>
       </c>
       <c r="B4" t="n">
         <v>408</v>
@@ -564,6 +562,38 @@
       <c r="H4" t="inlineStr">
         <is>
           <t>2025-08-20T08:55:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>79174463</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>40</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2025-08-20T09:36:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174460 (Cash) 2025-08-20T09:41:48
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,10 +566,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>79174463</t>
-        </is>
+      <c r="A5" t="n">
+        <v>79174463</v>
       </c>
       <c r="B5" t="n">
         <v>40</v>
@@ -594,6 +592,38 @@
       <c r="H5" t="inlineStr">
         <is>
           <t>2025-08-20T09:36:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>79174460</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>50</v>
+      </c>
+      <c r="C6" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025-08-20T09:41:48</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174449 (Cash) 2025-08-20T09:46:10
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,10 +596,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>79174460</t>
-        </is>
+      <c r="A6" t="n">
+        <v>79174460</v>
       </c>
       <c r="B6" t="n">
         <v>50</v>
@@ -624,6 +622,38 @@
       <c r="H6" t="inlineStr">
         <is>
           <t>2025-08-20T09:41:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>79174449</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>70</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>70</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2025-08-20T09:46:10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Reset payments.xlsx (clear all data)
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,188 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>76442711</v>
-      </c>
-      <c r="B2" t="n">
-        <v>408</v>
-      </c>
-      <c r="C2" t="n">
-        <v>61.2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>346.8</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2025-08-20T08:52:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>76442781</v>
-      </c>
-      <c r="B3" t="n">
-        <v>4080</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>4080</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2025-08-20T08:53:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>76442781</v>
-      </c>
-      <c r="B4" t="n">
-        <v>408</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>40</v>
-      </c>
-      <c r="E4" t="n">
-        <v>500</v>
-      </c>
-      <c r="F4" t="n">
-        <v>368</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Check</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2025-08-20T08:55:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>79174463</v>
-      </c>
-      <c r="B5" t="n">
-        <v>40</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>40</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2025-08-20T09:36:16</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>79174460</v>
-      </c>
-      <c r="B6" t="n">
-        <v>50</v>
-      </c>
-      <c r="C6" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>42.5</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2025-08-20T09:41:48</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>79174449</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>70</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>70</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>2025-08-20T09:46:10</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-21T07:35:23
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,38 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>50</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:35:23</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-23T09:26:33
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,10 +476,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A2" t="n">
+        <v>79174445</v>
       </c>
       <c r="B2" t="n">
         <v>50</v>
@@ -504,6 +502,38 @@
       <c r="H2" t="inlineStr">
         <is>
           <t>2025-08-21T07:35:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>25</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-08-23T09:26:33</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-23T09:33:22
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,10 +506,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A3" t="n">
+        <v>79174445</v>
       </c>
       <c r="B3" t="n">
         <v>25</v>
@@ -534,6 +532,38 @@
       <c r="H3" t="inlineStr">
         <is>
           <t>2025-08-23T09:26:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-08-23T09:33:22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-23T09:41:10
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,10 +536,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A4" t="n">
+        <v>79174445</v>
       </c>
       <c r="B4" t="n">
         <v>100</v>
@@ -564,6 +562,38 @@
       <c r="H4" t="inlineStr">
         <is>
           <t>2025-08-23T09:33:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3000</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2025-08-23T09:41:10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-23T09:41:43
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,10 +566,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A5" t="n">
+        <v>79174445</v>
       </c>
       <c r="B5" t="n">
         <v>3000</v>
@@ -594,6 +592,38 @@
       <c r="H5" t="inlineStr">
         <is>
           <t>2025-08-23T09:41:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025-08-23T09:41:43</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-29T16:20:43
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,10 +596,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A6" t="n">
+        <v>79174445</v>
       </c>
       <c r="B6" t="n">
         <v>5000</v>
@@ -624,6 +622,38 @@
       <c r="H6" t="inlineStr">
         <is>
           <t>2025-08-23T09:41:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2025-08-29T16:20:43</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add payment 79174445 (Cash) 2025-08-29T16:21:46
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,10 +626,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A7" t="n">
+        <v>79174445</v>
       </c>
       <c r="B7" t="n">
         <v>5</v>
@@ -654,6 +652,38 @@
       <c r="H7" t="inlineStr">
         <is>
           <t>2025-08-29T16:20:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2025-08-29T16:21:46</t>
         </is>
       </c>
     </row>

</xml_diff>